<commit_message>
Adaptive cow placement and movement
</commit_message>
<xml_diff>
--- a/rules.xlsx
+++ b/rules.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t xml:space="preserve">Type of Food</t>
   </si>
@@ -46,16 +46,31 @@
     <t xml:space="preserve">Result</t>
   </si>
   <si>
+    <t xml:space="preserve">Dimensions</t>
+  </si>
+  <si>
     <t xml:space="preserve">Grass</t>
   </si>
   <si>
     <t xml:space="preserve">green</t>
   </si>
   <si>
+    <t xml:space="preserve">Square_Lenght</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpha</t>
+  </si>
+  <si>
     <t xml:space="preserve">Corn</t>
   </si>
   <si>
     <t xml:space="preserve">yellow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(dim_box + self.spacing) </t>
   </si>
   <si>
     <t xml:space="preserve">Soybean</t>
@@ -98,11 +113,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -125,6 +141,12 @@
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -169,20 +191,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,217 +403,291 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.92"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="34.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="true" ht="34.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="n">
         <v>0.8</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <f aca="false">C2*H2*MIN(F2:F6)</f>
         <v>150</v>
       </c>
+      <c r="K2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="0" t="n">
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <f aca="false">C3*H3*MIN(F2:F6)</f>
         <v>8</v>
       </c>
+      <c r="K3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="0" t="n">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="n">
         <v>0.65</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="1" t="n">
         <f aca="false">C4*H4*MIN(F2:F6)</f>
         <v>36</v>
       </c>
+      <c r="K4" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="0" t="n">
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="n">
         <v>0.3</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="1" t="n">
         <f aca="false">C5*H5*MIN(F2:F6)</f>
         <v>48</v>
       </c>
+      <c r="K5" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="0" t="n">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="0" t="n">
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="1" t="n">
         <f aca="false">C6*H6*MIN(F2:F6)</f>
         <v>70</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>19</v>
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="0" t="n">
+      <c r="H8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="1" t="n">
         <f aca="false">AVERAGE(I2:I6)</f>
         <v>62.4</v>
       </c>
+      <c r="K8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="0" t="n">
+      <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="1" t="n">
         <f aca="false">I8*100</f>
         <v>6240</v>
       </c>
+      <c r="K9" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K10" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K12" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="K1:M1"/>
     <mergeCell ref="B7:D7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>